<commit_message>
error prop to do
</commit_message>
<xml_diff>
--- a/Lab 5/Lab_LED.xlsx
+++ b/Lab 5/Lab_LED.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\School\20189-W-McGill\PHYS258\phys-258-coding\Lab 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12864" windowHeight="8592"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
   <si>
     <t>Red</t>
   </si>
@@ -114,6 +114,21 @@
   </si>
   <si>
     <t xml:space="preserve">TRUE </t>
+  </si>
+  <si>
+    <t>AVG h per color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERR </t>
+  </si>
+  <si>
+    <t>RIP nop</t>
+  </si>
+  <si>
+    <t>std dev</t>
+  </si>
+  <si>
+    <t>Half-width</t>
   </si>
 </sst>
 </file>
@@ -456,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG19"/>
+  <dimension ref="A1:AL19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,14 +482,16 @@
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.5546875" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="12" customWidth="1"/>
+    <col min="37" max="38" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -494,11 +511,11 @@
         <f>D1/B1</f>
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -509,21 +526,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>20</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>22</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -539,50 +556,59 @@
       <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="J5" t="s">
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" t="s">
         <v>4</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>7</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>13</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>4</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>7</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>13</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>14</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>4</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>7</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>13</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>14</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI5" t="s">
         <v>23</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AJ5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -597,96 +623,116 @@
         <v>1.0029999999999999</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:F15" si="0">C6-D6</f>
+        <f t="shared" ref="E6:E15" si="0">C6-D6</f>
         <v>1.8150000000000002</v>
       </c>
       <c r="F6">
         <v>626.69000000000005</v>
       </c>
       <c r="G6">
+        <f>12.64/2</f>
+        <v>6.32</v>
+      </c>
+      <c r="H6">
         <f>E6/(3*(10^8))*1.602*10^(-19)*($F6*10^(-9))</f>
         <v>6.0739421490000004E-34</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>0</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1.0089999999999999</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>2.8119999999999998</v>
       </c>
-      <c r="L6">
-        <f>J6*$F$1</f>
+      <c r="M6">
+        <f t="shared" ref="M6:M15" si="1">K6*$F$1</f>
         <v>1.0089999999999999</v>
       </c>
-      <c r="M6">
-        <f t="shared" ref="M6:M15" si="1">K6-L6</f>
+      <c r="N6">
+        <f t="shared" ref="N6:N15" si="2">L6-M6</f>
         <v>1.8029999999999999</v>
       </c>
-      <c r="N6">
-        <f>M6/(3*(10^8))*1.602*10^(-19)*($F6*10^(-9))</f>
+      <c r="O6">
+        <f>N6/(3*(10^8))*1.602*10^(-19)*($F6*10^(-9))</f>
         <v>6.0337838538000006E-34</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>0</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>0.997</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>2.8050000000000002</v>
       </c>
-      <c r="S6">
-        <f>Q6*$F$1</f>
+      <c r="T6">
+        <f t="shared" ref="T6:T15" si="3">R6*$F$1</f>
         <v>0.997</v>
       </c>
-      <c r="T6">
-        <f t="shared" ref="T6:T15" si="2">R6-S6</f>
+      <c r="U6">
+        <f t="shared" ref="U6:U15" si="4">S6-T6</f>
         <v>1.8080000000000003</v>
       </c>
-      <c r="U6">
-        <f>T6/(3*(10^8))*1.602*10^(-19)*($F6*10^(-9))</f>
+      <c r="V6">
+        <f>U6/(3*(10^8))*1.602*10^(-19)*($F6*10^(-9))</f>
         <v>6.0505164768000018E-34</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>0</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>1.01</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>2.8260000000000001</v>
       </c>
-      <c r="Z6">
-        <f>X6*$F$1</f>
+      <c r="AA6">
+        <f t="shared" ref="AA6:AA15" si="5">Y6*$F$1</f>
         <v>1.01</v>
       </c>
-      <c r="AA6">
-        <f t="shared" ref="AA6:AA15" si="3">Y6-Z6</f>
+      <c r="AB6">
+        <f t="shared" ref="AB6:AB15" si="6">Z6-AA6</f>
         <v>1.8160000000000001</v>
       </c>
-      <c r="AB6">
-        <f>AA6/(3*(10^8))*1.602*10^(-19)*($F6*10^(-9))</f>
+      <c r="AC6">
+        <f>AB6/(3*(10^8))*1.602*10^(-19)*($F6*10^(-9))</f>
         <v>6.0772886736000017E-34</v>
       </c>
-      <c r="AD6">
-        <f>AVERAGE(AA6,T6, M6, E6)</f>
+      <c r="AE6">
+        <f>AVERAGE(AC6,V6,O6,H6)</f>
+        <v>6.0588827883000016E-34</v>
+      </c>
+      <c r="AF6">
+        <f>_xlfn.STDEV.S(AC6,V6,O6,H6)</f>
+        <v>2.0538684147398526E-36</v>
+      </c>
+      <c r="AG6">
+        <f>(AF6)^(-2)</f>
+        <v>2.3705808273383635E+71</v>
+      </c>
+      <c r="AH6">
+        <f>AG6*AE6</f>
+        <v>1.4363071373034389E+38</v>
+      </c>
+      <c r="AI6">
+        <f t="shared" ref="AI6:AI15" si="7">AVERAGE(AB6,U6, N6, E6)</f>
         <v>1.8105000000000002</v>
       </c>
-      <c r="AE6">
+      <c r="AJ6">
         <v>630</v>
       </c>
-      <c r="AF6">
-        <f>AD6/(3*(10^8))*1.602*10^(-19)*(AE6*10^(-9))</f>
+      <c r="AK6">
+        <f>AI6/(3*(10^8))*1.602*10^(-19)*(AJ6*10^(-9))</f>
         <v>6.0908841000000014E-34</v>
       </c>
-      <c r="AG6">
-        <f>_xlfn.STDEV.S(AA6,T6, M6, E6)</f>
+      <c r="AL6">
+        <f t="shared" ref="AL6:AL12" si="8">_xlfn.STDEV.S(AB6,U6, N6, E6)</f>
         <v>6.1373175465073704E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -697,78 +743,78 @@
         <v>3.7130000000000001</v>
       </c>
       <c r="D7">
-        <f>B7*$F$1</f>
+        <f t="shared" ref="D6:D15" si="9">B7*$F$1</f>
         <v>1.018</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
         <v>2.6950000000000003</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>2</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>1.008</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>3.6960000000000002</v>
-      </c>
-      <c r="L7">
-        <f>J7*$F$1</f>
-        <v>1.008</v>
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
+        <v>1.008</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
         <v>2.6880000000000002</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>2</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>0.999</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>3.69</v>
       </c>
-      <c r="S7">
-        <f>Q7*$F$1</f>
+      <c r="T7">
+        <f t="shared" si="3"/>
         <v>0.999</v>
       </c>
-      <c r="T7">
-        <f t="shared" si="2"/>
+      <c r="U7">
+        <f t="shared" si="4"/>
         <v>2.6909999999999998</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>2</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>1</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>3.6909999999999998</v>
       </c>
-      <c r="Z7">
-        <f>X7*$F$1</f>
+      <c r="AA7">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="AA7">
-        <f t="shared" si="3"/>
+      <c r="AB7">
+        <f t="shared" si="6"/>
         <v>2.6909999999999998</v>
       </c>
-      <c r="AD7">
-        <f>AVERAGE(AA7,T7, M7, E7)</f>
+      <c r="AI7">
+        <f t="shared" si="7"/>
         <v>2.6912500000000001</v>
       </c>
-      <c r="AF7">
-        <f t="shared" ref="AF7:AF12" si="4">AD7/(3*(10^8))*1.602*10^(-19)*(AE7*10^(-9))</f>
+      <c r="AK7">
+        <f t="shared" ref="AK7:AK12" si="10">AI7/(3*(10^8))*1.602*10^(-19)*(AJ7*10^(-9))</f>
         <v>0</v>
       </c>
-      <c r="AG7">
-        <f>_xlfn.STDEV.S(AA7,T7, M7, E7)</f>
+      <c r="AL7">
+        <f t="shared" si="8"/>
         <v>2.8722813232690846E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -779,7 +825,7 @@
         <v>2.8570000000000002</v>
       </c>
       <c r="D8">
-        <f>B8*$F$1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E8">
@@ -790,89 +836,109 @@
         <v>606.47</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G13" si="5">E8/(3*(10^8))*1.602*10^(-19)*($F8*10^(-9))</f>
+        <f>16.33/2</f>
+        <v>8.1649999999999991</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ref="H8:H13" si="11">E8/(3*(10^8))*1.602*10^(-19)*($F8*10^(-9))</f>
         <v>6.013986978600001E-34</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>5</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>0.999</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>2.8490000000000002</v>
-      </c>
-      <c r="L8">
-        <f>J8*$F$1</f>
-        <v>0.999</v>
       </c>
       <c r="M8">
         <f t="shared" si="1"/>
+        <v>0.999</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
         <v>1.85</v>
       </c>
-      <c r="N8">
-        <f t="shared" ref="N7:N13" si="6">M8/(3*(10^8))*1.602*10^(-19)*($F8*10^(-9))</f>
+      <c r="O8">
+        <f t="shared" ref="O8:O13" si="12">N8/(3*(10^8))*1.602*10^(-19)*($F8*10^(-9))</f>
         <v>5.9913171300000018E-34</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>5</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>1.0069999999999999</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>2.859</v>
       </c>
-      <c r="S8">
-        <f>Q8*$F$1</f>
+      <c r="T8">
+        <f t="shared" si="3"/>
         <v>1.0069999999999999</v>
       </c>
-      <c r="T8">
-        <f t="shared" si="2"/>
+      <c r="U8">
+        <f t="shared" si="4"/>
         <v>1.8520000000000001</v>
       </c>
-      <c r="U8">
-        <f t="shared" ref="U7:U13" si="7">T8/(3*(10^8))*1.602*10^(-19)*($F8*10^(-9))</f>
+      <c r="V8">
+        <f t="shared" ref="V8:V13" si="13">U8/(3*(10^8))*1.602*10^(-19)*($F8*10^(-9))</f>
         <v>5.9977942295999999E-34</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>5</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>1.0029999999999999</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>2.86</v>
       </c>
-      <c r="Z8">
-        <f>X8*$F$1</f>
+      <c r="AA8">
+        <f t="shared" si="5"/>
         <v>1.0029999999999999</v>
       </c>
-      <c r="AA8">
-        <f t="shared" si="3"/>
+      <c r="AB8">
+        <f t="shared" si="6"/>
         <v>1.857</v>
       </c>
-      <c r="AB8">
-        <f t="shared" ref="AB7:AB13" si="8">AA8/(3*(10^8))*1.602*10^(-19)*($F8*10^(-9))</f>
+      <c r="AC8">
+        <f t="shared" ref="AC8:AC13" si="14">AB8/(3*(10^8))*1.602*10^(-19)*($F8*10^(-9))</f>
         <v>6.013986978600001E-34</v>
       </c>
-      <c r="AD8">
-        <f>AVERAGE(AA8,T8, M8, E8)</f>
+      <c r="AE8">
+        <f t="shared" ref="AE8:AE13" si="15">AVERAGE(AC8,V8,O8,H8)</f>
+        <v>6.0042713292000005E-34</v>
+      </c>
+      <c r="AF8">
+        <f t="shared" ref="AF8:AF13" si="16">_xlfn.STDEV.S(AC8,V8,O8,H8)</f>
+        <v>1.1526083212566696E-36</v>
+      </c>
+      <c r="AG8">
+        <f t="shared" ref="AG8:AG13" si="17">(AF8)^(-2)</f>
+        <v>7.5272527446985575E+71</v>
+      </c>
+      <c r="AH8">
+        <f t="shared" ref="AH8:AH13" si="18">AG8*AE8</f>
+        <v>4.5195667842635559E+38</v>
+      </c>
+      <c r="AI8">
+        <f t="shared" si="7"/>
         <v>1.8540000000000001</v>
       </c>
-      <c r="AE8">
+      <c r="AJ8">
         <v>617</v>
       </c>
-      <c r="AF8">
-        <f t="shared" si="4"/>
+      <c r="AK8">
+        <f t="shared" si="10"/>
         <v>6.1085221200000021E-34</v>
       </c>
-      <c r="AG8">
-        <f>_xlfn.STDEV.S(AA8,T8, M8, E8)</f>
+      <c r="AL8">
+        <f t="shared" si="8"/>
         <v>3.5590260840104404E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -883,7 +949,7 @@
         <v>2.88</v>
       </c>
       <c r="D9">
-        <f>B9*$F$1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E9">
@@ -894,89 +960,109 @@
         <v>588.54999999999995</v>
       </c>
       <c r="G9">
-        <f t="shared" si="5"/>
+        <f>11.47/2</f>
+        <v>5.7350000000000003</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="11"/>
         <v>5.9085711600000001E-34</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>6</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>1.0009999999999999</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>2.8730000000000002</v>
-      </c>
-      <c r="L9">
-        <f>J9*$F$1</f>
-        <v>1.0009999999999999</v>
       </c>
       <c r="M9">
         <f t="shared" si="1"/>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="2"/>
         <v>1.8720000000000003</v>
       </c>
-      <c r="N9">
+      <c r="O9">
+        <f t="shared" si="12"/>
+        <v>5.8834283040000002E-34</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="S9">
+        <v>2.8730000000000002</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="3"/>
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="4"/>
+        <v>1.8800000000000003</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="13"/>
+        <v>5.908571160000001E-34</v>
+      </c>
+      <c r="X9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y9">
+        <v>0.998</v>
+      </c>
+      <c r="Z9">
+        <v>2.8759999999999999</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="5"/>
+        <v>0.998</v>
+      </c>
+      <c r="AB9">
         <f t="shared" si="6"/>
-        <v>5.8834283040000002E-34</v>
-      </c>
-      <c r="P9" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q9">
-        <v>0.99299999999999999</v>
-      </c>
-      <c r="R9">
-        <v>2.8730000000000002</v>
-      </c>
-      <c r="S9">
-        <f>Q9*$F$1</f>
-        <v>0.99299999999999999</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="2"/>
-        <v>1.8800000000000003</v>
-      </c>
-      <c r="U9">
+        <v>1.8779999999999999</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="14"/>
+        <v>5.9022854459999993E-34</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" si="15"/>
+        <v>5.9007140174999999E-34</v>
+      </c>
+      <c r="AF9">
+        <f t="shared" si="16"/>
+        <v>1.1898664564637986E-36</v>
+      </c>
+      <c r="AG9">
+        <f t="shared" si="17"/>
+        <v>7.063233392448323E+71</v>
+      </c>
+      <c r="AH9">
+        <f t="shared" si="18"/>
+        <v>4.1678120287693895E+38</v>
+      </c>
+      <c r="AI9">
         <f t="shared" si="7"/>
-        <v>5.908571160000001E-34</v>
-      </c>
-      <c r="W9" t="s">
-        <v>6</v>
-      </c>
-      <c r="X9">
-        <v>0.998</v>
-      </c>
-      <c r="Y9">
-        <v>2.8759999999999999</v>
-      </c>
-      <c r="Z9">
-        <f>X9*$F$1</f>
-        <v>0.998</v>
-      </c>
-      <c r="AA9">
-        <f t="shared" si="3"/>
-        <v>1.8779999999999999</v>
-      </c>
-      <c r="AB9">
+        <v>1.8775000000000002</v>
+      </c>
+      <c r="AJ9">
+        <v>590</v>
+      </c>
+      <c r="AK9">
+        <f t="shared" si="10"/>
+        <v>5.9152515000000012E-34</v>
+      </c>
+      <c r="AL9">
         <f t="shared" si="8"/>
-        <v>5.9022854459999993E-34</v>
-      </c>
-      <c r="AD9">
-        <f>AVERAGE(AA9,T9, M9, E9)</f>
-        <v>1.8775000000000002</v>
-      </c>
-      <c r="AE9">
-        <v>590</v>
-      </c>
-      <c r="AF9">
-        <f t="shared" si="4"/>
-        <v>5.9152515000000012E-34</v>
-      </c>
-      <c r="AG9">
-        <f>_xlfn.STDEV.S(AA9,T9, M9, E9)</f>
         <v>3.7859388972000681E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -987,7 +1073,7 @@
         <v>2.879</v>
       </c>
       <c r="D10">
-        <f>B10*$F$1</f>
+        <f t="shared" si="9"/>
         <v>1.0009999999999999</v>
       </c>
       <c r="E10">
@@ -998,86 +1084,106 @@
         <v>566.41999999999996</v>
       </c>
       <c r="G10">
-        <f t="shared" si="5"/>
+        <f>29.07/2</f>
+        <v>14.535</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="11"/>
         <v>5.6803542984000001E-34</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>8</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1.002</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>2.87</v>
-      </c>
-      <c r="L10">
-        <f>J10*$F$1</f>
-        <v>1.002</v>
       </c>
       <c r="M10">
         <f t="shared" si="1"/>
+        <v>1.002</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="2"/>
         <v>1.8680000000000001</v>
       </c>
-      <c r="N10">
+      <c r="O10">
+        <f t="shared" si="12"/>
+        <v>5.6501074704000001E-34</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="S10">
+        <v>2.8719999999999999</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="3"/>
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="4"/>
+        <v>1.8779999999999999</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="13"/>
+        <v>5.6803542984000001E-34</v>
+      </c>
+      <c r="X10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y10">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="Z10">
+        <v>2.8740000000000001</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="5"/>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="AB10">
         <f t="shared" si="6"/>
-        <v>5.6501074704000001E-34</v>
-      </c>
-      <c r="P10" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q10">
-        <v>0.99399999999999999</v>
-      </c>
-      <c r="R10">
-        <v>2.8719999999999999</v>
-      </c>
-      <c r="S10">
-        <f>Q10*$F$1</f>
-        <v>0.99399999999999999</v>
-      </c>
-      <c r="T10">
-        <f t="shared" si="2"/>
-        <v>1.8779999999999999</v>
-      </c>
-      <c r="U10">
+        <v>1.8730000000000002</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" si="14"/>
+        <v>5.6652308844000014E-34</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="15"/>
+        <v>5.6690117379E-34</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" si="16"/>
+        <v>1.4479566525421618E-36</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="17"/>
+        <v>4.7696760003698675E+71</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" si="18"/>
+        <v>2.7039349232076704E+38</v>
+      </c>
+      <c r="AI10">
         <f t="shared" si="7"/>
-        <v>5.6803542984000001E-34</v>
-      </c>
-      <c r="W10" t="s">
-        <v>8</v>
-      </c>
-      <c r="X10">
-        <v>1.0009999999999999</v>
-      </c>
-      <c r="Y10">
-        <v>2.8740000000000001</v>
-      </c>
-      <c r="Z10">
-        <f>X10*$F$1</f>
-        <v>1.0009999999999999</v>
-      </c>
-      <c r="AA10">
-        <f t="shared" si="3"/>
-        <v>1.8730000000000002</v>
-      </c>
-      <c r="AB10">
+        <v>1.8742500000000002</v>
+      </c>
+      <c r="AK10">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AL10">
         <f t="shared" si="8"/>
-        <v>5.6652308844000014E-34</v>
-      </c>
-      <c r="AD10">
-        <f>AVERAGE(AA10,T10, M10, E10)</f>
-        <v>1.8742500000000002</v>
-      </c>
-      <c r="AF10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AG10">
-        <f>_xlfn.STDEV.S(AA10,T10, M10, E10)</f>
         <v>4.7871355387816266E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1088,7 +1194,7 @@
         <v>3.3580000000000001</v>
       </c>
       <c r="D11">
-        <f>B11*$F$1</f>
+        <f t="shared" si="9"/>
         <v>1.0089999999999999</v>
       </c>
       <c r="E11">
@@ -1099,89 +1205,109 @@
         <v>533.88</v>
       </c>
       <c r="G11">
-        <f t="shared" si="5"/>
+        <f>33.22/2</f>
+        <v>16.61</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="11"/>
         <v>6.6968092008000023E-34</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>10</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>1.0009999999999999</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>3.35</v>
-      </c>
-      <c r="L11">
-        <f>J11*$F$1</f>
-        <v>1.0009999999999999</v>
       </c>
       <c r="M11">
         <f t="shared" si="1"/>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="2"/>
         <v>2.3490000000000002</v>
       </c>
-      <c r="N11">
+      <c r="O11">
+        <f t="shared" si="12"/>
+        <v>6.6968092008000023E-34</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>10</v>
+      </c>
+      <c r="R11">
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="S11">
+        <v>3.363</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="3"/>
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="4"/>
+        <v>2.3540000000000001</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="13"/>
+        <v>6.7110637968000011E-34</v>
+      </c>
+      <c r="X11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y11">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="Z11">
+        <v>3.3559999999999999</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="5"/>
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="AB11">
         <f t="shared" si="6"/>
-        <v>6.6968092008000023E-34</v>
-      </c>
-      <c r="P11" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q11">
-        <v>1.0089999999999999</v>
-      </c>
-      <c r="R11">
-        <v>3.363</v>
-      </c>
-      <c r="S11">
-        <f>Q11*$F$1</f>
-        <v>1.0089999999999999</v>
-      </c>
-      <c r="T11">
-        <f t="shared" si="2"/>
-        <v>2.3540000000000001</v>
-      </c>
-      <c r="U11">
+        <v>2.3529999999999998</v>
+      </c>
+      <c r="AC11">
+        <f t="shared" si="14"/>
+        <v>6.7082128775999998E-34</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" si="15"/>
+        <v>6.7032237690000018E-34</v>
+      </c>
+      <c r="AF11">
+        <f t="shared" si="16"/>
+        <v>7.4977910283012678E-37</v>
+      </c>
+      <c r="AG11">
+        <f t="shared" si="17"/>
+        <v>1.7788254568264595E+72</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" si="18"/>
+        <v>1.192386508310141E+39</v>
+      </c>
+      <c r="AI11">
         <f t="shared" si="7"/>
-        <v>6.7110637968000011E-34</v>
-      </c>
-      <c r="W11" t="s">
-        <v>10</v>
-      </c>
-      <c r="X11">
-        <v>1.0029999999999999</v>
-      </c>
-      <c r="Y11">
-        <v>3.3559999999999999</v>
-      </c>
-      <c r="Z11">
-        <f>X11*$F$1</f>
-        <v>1.0029999999999999</v>
-      </c>
-      <c r="AA11">
-        <f t="shared" si="3"/>
-        <v>2.3529999999999998</v>
-      </c>
-      <c r="AB11">
+        <v>2.3512500000000003</v>
+      </c>
+      <c r="AJ11">
+        <v>565</v>
+      </c>
+      <c r="AK11">
+        <f t="shared" si="10"/>
+        <v>7.0939563750000014E-34</v>
+      </c>
+      <c r="AL11">
         <f t="shared" si="8"/>
-        <v>6.7082128775999998E-34</v>
-      </c>
-      <c r="AD11">
-        <f>AVERAGE(AA11,T11, M11, E11)</f>
-        <v>2.3512500000000003</v>
-      </c>
-      <c r="AE11">
-        <v>565</v>
-      </c>
-      <c r="AF11">
-        <f t="shared" si="4"/>
-        <v>7.0939563750000014E-34</v>
-      </c>
-      <c r="AG11">
-        <f>_xlfn.STDEV.S(AA11,T11, M11, E11)</f>
         <v>2.6299556396764483E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1192,7 +1318,7 @@
         <v>3.641</v>
       </c>
       <c r="D12">
-        <f>B12*$F$1</f>
+        <f t="shared" si="9"/>
         <v>1.0049999999999999</v>
       </c>
       <c r="E12">
@@ -1203,89 +1329,109 @@
         <v>462.14</v>
       </c>
       <c r="G12">
-        <f t="shared" si="5"/>
+        <f>19.59/2</f>
+        <v>9.7949999999999999</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="11"/>
         <v>6.505193553600001E-34</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>11</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.998</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>3.6309999999999998</v>
-      </c>
-      <c r="L12">
-        <f>J12*$F$1</f>
-        <v>0.998</v>
       </c>
       <c r="M12">
         <f t="shared" si="1"/>
+        <v>0.998</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="2"/>
         <v>2.633</v>
       </c>
-      <c r="N12">
+      <c r="O12">
+        <f t="shared" si="12"/>
+        <v>6.497790070800001E-34</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>11</v>
+      </c>
+      <c r="R12">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="S12">
+        <v>3.6440000000000001</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="3"/>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="4"/>
+        <v>2.6390000000000002</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="13"/>
+        <v>6.5125970364000011E-34</v>
+      </c>
+      <c r="X12" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y12">
+        <v>1.008</v>
+      </c>
+      <c r="Z12">
+        <v>3.645</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="5"/>
+        <v>1.008</v>
+      </c>
+      <c r="AB12">
         <f t="shared" si="6"/>
-        <v>6.497790070800001E-34</v>
-      </c>
-      <c r="P12" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q12">
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="R12">
-        <v>3.6440000000000001</v>
-      </c>
-      <c r="S12">
-        <f>Q12*$F$1</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="2"/>
-        <v>2.6390000000000002</v>
-      </c>
-      <c r="U12">
+        <v>2.637</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="14"/>
+        <v>6.5076613811999999E-34</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="15"/>
+        <v>6.5058105105000009E-34</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="16"/>
+        <v>6.1695689999999274E-37</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="17"/>
+        <v>2.6271831413725875E+72</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="18"/>
+        <v>1.7091955694150189E+39</v>
+      </c>
+      <c r="AI12">
         <f t="shared" si="7"/>
-        <v>6.5125970364000011E-34</v>
-      </c>
-      <c r="W12" t="s">
-        <v>11</v>
-      </c>
-      <c r="X12">
-        <v>1.008</v>
-      </c>
-      <c r="Y12">
-        <v>3.645</v>
-      </c>
-      <c r="Z12">
-        <f>X12*$F$1</f>
-        <v>1.008</v>
-      </c>
-      <c r="AA12">
-        <f t="shared" si="3"/>
-        <v>2.637</v>
-      </c>
-      <c r="AB12">
+        <v>2.63625</v>
+      </c>
+      <c r="AJ12">
+        <v>465</v>
+      </c>
+      <c r="AK12">
+        <f t="shared" si="10"/>
+        <v>6.546072375000001E-34</v>
+      </c>
+      <c r="AL12">
         <f t="shared" si="8"/>
-        <v>6.5076613811999999E-34</v>
-      </c>
-      <c r="AD12">
-        <f>AVERAGE(AA12,T12, M12, E12)</f>
-        <v>2.63625</v>
-      </c>
-      <c r="AE12">
-        <v>465</v>
-      </c>
-      <c r="AF12">
-        <f t="shared" si="4"/>
-        <v>6.546072375000001E-34</v>
-      </c>
-      <c r="AG12">
-        <f>_xlfn.STDEV.S(AA12,T12, M12, E12)</f>
         <v>2.5000000000000798E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1296,7 +1442,7 @@
         <v>4.0019999999999998</v>
       </c>
       <c r="D13">
-        <f>B13*$F$1</f>
+        <f t="shared" si="9"/>
         <v>1.004</v>
       </c>
       <c r="E13">
@@ -1307,78 +1453,98 @@
         <v>399.26</v>
       </c>
       <c r="G13">
-        <f t="shared" si="5"/>
+        <f>10.28/2</f>
+        <v>5.14</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="11"/>
         <v>6.3918811031999996E-34</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>15</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>1.004</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>4</v>
-      </c>
-      <c r="L13">
-        <f>J13*$F$1</f>
-        <v>1.004</v>
       </c>
       <c r="M13">
         <f t="shared" si="1"/>
+        <v>1.004</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
         <v>2.996</v>
       </c>
-      <c r="N13">
+      <c r="O13">
+        <f t="shared" si="12"/>
+        <v>6.3876170064000005E-34</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>15</v>
+      </c>
+      <c r="R13">
+        <v>1.008</v>
+      </c>
+      <c r="S13">
+        <v>4.0119999999999996</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="3"/>
+        <v>1.008</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="4"/>
+        <v>3.0039999999999996</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="13"/>
+        <v>6.4046733935999997E-34</v>
+      </c>
+      <c r="X13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y13">
+        <v>1.014</v>
+      </c>
+      <c r="Z13">
+        <v>4.0129999999999999</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="5"/>
+        <v>1.014</v>
+      </c>
+      <c r="AB13">
         <f t="shared" si="6"/>
-        <v>6.3876170064000005E-34</v>
-      </c>
-      <c r="P13" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q13">
-        <v>1.008</v>
-      </c>
-      <c r="R13">
-        <v>4.0119999999999996</v>
-      </c>
-      <c r="S13">
-        <f>Q13*$F$1</f>
-        <v>1.008</v>
-      </c>
-      <c r="T13">
-        <f t="shared" si="2"/>
-        <v>3.0039999999999996</v>
-      </c>
-      <c r="U13">
+        <v>2.9989999999999997</v>
+      </c>
+      <c r="AC13">
+        <f t="shared" si="14"/>
+        <v>6.3940131515999996E-34</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="15"/>
+        <v>6.394546163699999E-34</v>
+      </c>
+      <c r="AF13">
+        <f t="shared" si="16"/>
+        <v>7.2562767243950931E-37</v>
+      </c>
+      <c r="AG13">
+        <f t="shared" si="17"/>
+        <v>1.8992071073956291E+72</v>
+      </c>
+      <c r="AH13">
+        <f t="shared" si="18"/>
+        <v>1.2144567522668492E+39</v>
+      </c>
+      <c r="AI13">
         <f t="shared" si="7"/>
-        <v>6.4046733935999997E-34</v>
-      </c>
-      <c r="W13" t="s">
-        <v>15</v>
-      </c>
-      <c r="X13">
-        <v>1.014</v>
-      </c>
-      <c r="Y13">
-        <v>4.0129999999999999</v>
-      </c>
-      <c r="Z13">
-        <f>X13*$F$1</f>
-        <v>1.014</v>
-      </c>
-      <c r="AA13">
-        <f t="shared" si="3"/>
-        <v>2.9989999999999997</v>
-      </c>
-      <c r="AB13">
-        <f t="shared" si="8"/>
-        <v>6.3940131515999996E-34</v>
-      </c>
-      <c r="AD13">
-        <f>AVERAGE(AA13,T13, M13, E13)</f>
         <v>2.9992499999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1389,70 +1555,70 @@
         <v>3.601</v>
       </c>
       <c r="D14">
-        <f>B14*$F$1</f>
+        <f t="shared" si="9"/>
         <v>1.0029999999999999</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
         <v>2.5979999999999999</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>16</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>0.999</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>3.605</v>
-      </c>
-      <c r="L14">
-        <f>J14*$F$1</f>
-        <v>0.999</v>
       </c>
       <c r="M14">
         <f t="shared" si="1"/>
+        <v>0.999</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="2"/>
         <v>2.6059999999999999</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>16</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>0.99299999999999999</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>3.5960000000000001</v>
       </c>
-      <c r="S14">
-        <f>Q14*$F$1</f>
+      <c r="T14">
+        <f t="shared" si="3"/>
         <v>0.99299999999999999</v>
       </c>
-      <c r="T14">
-        <f t="shared" si="2"/>
+      <c r="U14">
+        <f t="shared" si="4"/>
         <v>2.6030000000000002</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>16</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <v>1.0189999999999999</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>3.6240000000000001</v>
       </c>
-      <c r="Z14">
-        <f>X14*$F$1</f>
+      <c r="AA14">
+        <f t="shared" si="5"/>
         <v>1.0189999999999999</v>
       </c>
-      <c r="AA14">
-        <f t="shared" si="3"/>
+      <c r="AB14">
+        <f t="shared" si="6"/>
         <v>2.6050000000000004</v>
       </c>
-      <c r="AD14">
-        <f>AVERAGE(AA14,T14, M14, E14)</f>
+      <c r="AI14">
+        <f t="shared" si="7"/>
         <v>2.6029999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1463,108 +1629,125 @@
         <v>3.6619999999999999</v>
       </c>
       <c r="D15">
-        <f>B15*$F$1</f>
+        <f t="shared" si="9"/>
         <v>1.0069999999999999</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
         <v>2.6550000000000002</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>12</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>1.0109999999999999</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>3.6869999999999998</v>
-      </c>
-      <c r="L15">
-        <f>J15*$F$1</f>
-        <v>1.0109999999999999</v>
       </c>
       <c r="M15">
         <f t="shared" si="1"/>
+        <v>1.0109999999999999</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
         <v>2.6760000000000002</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>12</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>0.997</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>3.67</v>
       </c>
-      <c r="S15">
-        <f>Q15*$F$1</f>
+      <c r="T15">
+        <f t="shared" si="3"/>
         <v>0.997</v>
       </c>
-      <c r="T15">
-        <f t="shared" si="2"/>
+      <c r="U15">
+        <f t="shared" si="4"/>
         <v>2.673</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>12</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <v>1.0189999999999999</v>
       </c>
-      <c r="Y15">
+      <c r="Z15">
         <v>3.694</v>
       </c>
-      <c r="Z15">
-        <f>X15*$F$1</f>
+      <c r="AA15">
+        <f t="shared" si="5"/>
         <v>1.0189999999999999</v>
       </c>
-      <c r="AA15">
-        <f t="shared" si="3"/>
+      <c r="AB15">
+        <f t="shared" si="6"/>
         <v>2.6749999999999998</v>
       </c>
-      <c r="AD15">
-        <f>AVERAGE(AA15,T15, M15, E15)</f>
+      <c r="AI15">
+        <f t="shared" si="7"/>
         <v>2.6697500000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="AE16" t="s">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ16" t="s">
         <v>25</v>
       </c>
-      <c r="AF16">
-        <f>AVERAGE(AF12,AF11,AF9,AF8,AF6)</f>
+      <c r="AK16">
+        <f>AVERAGE(AK12,AK11,AK9,AK8,AK6)</f>
         <v>6.3509372940000016E-34</v>
       </c>
-      <c r="AG16">
-        <f>_xlfn.STDEV.S(AF12,AF11,AF9,AF8,AF6)</f>
+      <c r="AL16">
+        <f>_xlfn.STDEV.S(AK12,AK11,AK9,AK8,AK6)</f>
         <v>4.7601731742538087E-35</v>
       </c>
     </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:34" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
         <v>26</v>
       </c>
-      <c r="G17">
-        <f>AVERAGE(G6:G13,N6:N13,U6:U13,AB6:AB13)</f>
+      <c r="H17">
+        <f>AVERAGE(H6:H13,O6:O13,V6:V13,AC6:AC13)</f>
         <v>6.1766371880142865E-34</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>29</v>
       </c>
+      <c r="AF17" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG17">
+        <f>SUM(AH6:AH13)/SUM(AG6:AG13)</f>
+        <v>6.3677945859622569E-34</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:34" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
         <v>28</v>
       </c>
-      <c r="G18">
-        <f>_xlfn.STDEV.S(G6:G13,N6:N13,U6:U13,AB6:AB13)</f>
+      <c r="H18">
+        <f>_xlfn.STDEV.S(H6:H13,O6:O13,V6:V13,AC6:AC13)</f>
         <v>3.4669139878005411E-35</v>
       </c>
+      <c r="AF18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG18">
+        <f>SQRT(1/SUM(AG6:AG13))</f>
+        <v>3.4343603867601556E-37</v>
+      </c>
     </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:34" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>6.6259999999999998E-34</v>
       </c>
     </row>

</xml_diff>